<commit_message>
change judge dlock position
</commit_message>
<xml_diff>
--- a/Design/DoorLockCntr/test/Testcase/tc_DLockStatus.xlsx
+++ b/Design/DoorLockCntr/test/Testcase/tc_DLockStatus.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\Study\IncrementalTesting\tryIncrementalTest_Dlock\Design\DoorLockCntr\test\Testcase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\EVENT\EXPO\2023\Design\DoorLockCntr\test\Testcase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87410473-697E-46BC-BCAE-3910965F8898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E917FC5D-5C1C-4767-B5A0-E1CFB9556362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-2976" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testcase" sheetId="2" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:F15"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -501,10 +501,10 @@
         <v>0.1</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -581,10 +581,10 @@
         <v>0.5</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>